<commit_message>
Adding latest XL updates - graphs etc.
</commit_message>
<xml_diff>
--- a/node-api/PURE_REGULAR_TESTS_NODE.xlsx
+++ b/node-api/PURE_REGULAR_TESTS_NODE.xlsx
@@ -1,6 +1,6 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" mc:Ignorable="x15 xr xr6 xr10">
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10309"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
@@ -8,27 +8,13 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/chrisconnor/Sites/HONOURS_PROJECT/node-api/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:40009_{0112310E-2158-5040-A310-C2EA29846BE6}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C48E0324-6ED1-D946-A939-302CE69AD24A}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="460" windowWidth="51200" windowHeight="28340"/>
+    <workbookView xWindow="51200" yWindow="4500" windowWidth="38400" windowHeight="21140" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="PURE_REGULAR_TESTS_NODE" sheetId="1" r:id="rId1"/>
   </sheets>
-  <definedNames>
-    <definedName name="_xlchart.v1.0" hidden="1">PURE_REGULAR_TESTS_NODE!$B$203:$B$402</definedName>
-    <definedName name="_xlchart.v1.1" hidden="1">PURE_REGULAR_TESTS_NODE!$B$2:$B$202</definedName>
-    <definedName name="_xlchart.v1.10" hidden="1">PURE_REGULAR_TESTS_NODE!$B$2:$B$202</definedName>
-    <definedName name="_xlchart.v1.11" hidden="1">PURE_REGULAR_TESTS_NODE!$B$403:$B$603</definedName>
-    <definedName name="_xlchart.v1.2" hidden="1">PURE_REGULAR_TESTS_NODE!$B$403:$B$603</definedName>
-    <definedName name="_xlchart.v1.3" hidden="1">PURE_REGULAR_TESTS_NODE!$B$203:$B$402</definedName>
-    <definedName name="_xlchart.v1.4" hidden="1">PURE_REGULAR_TESTS_NODE!$B$2:$B$202</definedName>
-    <definedName name="_xlchart.v1.5" hidden="1">PURE_REGULAR_TESTS_NODE!$B$403:$B$603</definedName>
-    <definedName name="_xlchart.v1.6" hidden="1">PURE_REGULAR_TESTS_NODE!$B$203:$B$402</definedName>
-    <definedName name="_xlchart.v1.7" hidden="1">PURE_REGULAR_TESTS_NODE!$B$2:$B$202</definedName>
-    <definedName name="_xlchart.v1.8" hidden="1">PURE_REGULAR_TESTS_NODE!$B$403:$B$603</definedName>
-    <definedName name="_xlchart.v1.9" hidden="1">PURE_REGULAR_TESTS_NODE!$B$203:$B$402</definedName>
-  </definedNames>
   <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
@@ -80,7 +66,7 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <numFmts count="2">
     <numFmt numFmtId="164" formatCode="General&quot; MB&quot;"/>
     <numFmt numFmtId="165" formatCode="0&quot;ms&quot;"/>
@@ -4735,11 +4721,11 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:O603"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="K21" sqref="K21"/>
+      <selection activeCell="K12" sqref="K12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>
@@ -4995,6 +4981,10 @@
       <c r="E9" s="4">
         <v>70</v>
       </c>
+      <c r="J9">
+        <f>_xlfn.VAR.P(J4:J6)</f>
+        <v>8.5030002923802179</v>
+      </c>
     </row>
     <row r="10" spans="1:15">
       <c r="A10" s="4">
@@ -5028,6 +5018,14 @@
       </c>
       <c r="E11" s="4">
         <v>70</v>
+      </c>
+      <c r="J11" s="3">
+        <f>J4-J6</f>
+        <v>6.697213930348255</v>
+      </c>
+      <c r="K11" s="3">
+        <f>K4-K6</f>
+        <v>5.879999999999999</v>
       </c>
     </row>
     <row r="12" spans="1:15">

</xml_diff>